<commit_message>
Removed legacy loader calls from PropertyTests and fixed tests that had multiple representations.
Also added labels to help me reorganize the tests into appropriate test files/classes.

Files checked in: DataRepo/data/tests/small_obob2/serum_lactate_sample_table.xlsx DataRepo/tests/test_models.py DataRepo/data/tests/small_obob/animal_sample_table_labeled_elements_v3.xlsx
</commit_message>
<xml_diff>
--- a/DataRepo/data/tests/small_obob2/serum_lactate_sample_table.xlsx
+++ b/DataRepo/data/tests/small_obob2/serum_lactate_sample_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rleach/PROJECT-local/TRACEBASE/tracebase/DataRepo/data/tests/small_obob2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6475C57A-45E3-4D47-B22E-CF3FC09731B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B086026-595A-9646-A533-1EAB40CAFBA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3040" yWindow="6880" windowWidth="27640" windowHeight="16940" activeTab="5" xr2:uid="{76787519-8C47-6C44-9922-0A2F9B56DD8D}"/>
+    <workbookView xWindow="3040" yWindow="6880" windowWidth="27640" windowHeight="16940" activeTab="6" xr2:uid="{76787519-8C47-6C44-9922-0A2F9B56DD8D}"/>
   </bookViews>
   <sheets>
     <sheet name="Study" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,9 @@
     <sheet name="Animals" sheetId="2" r:id="rId4"/>
     <sheet name="Samples" sheetId="3" r:id="rId5"/>
     <sheet name="Sequences" sheetId="6" r:id="rId6"/>
+    <sheet name="Treatments" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="181029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -998,6 +999,47 @@
           </rPr>
           <t>Notes on this mass spectrometer run sequence.
 Must be unique.
+Optional.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>TraceBase Dev Team</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{E72B02AD-5C34-8B4B-977D-CD65C96BB91F}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Courier"/>
+            <family val="2"/>
+          </rPr>
+          <t>Unique name of the protocol.
+The values in this column are referenced by the 'Treatment' column in the
+'Animals' sheet.
+Must be unique.
+Required.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{46C7375F-C093-6448-ACEE-08B5115B2E97}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Courier"/>
+            <family val="2"/>
+          </rPr>
+          <t>Full text of the protocol's methods.
 Optional.</t>
         </r>
       </text>
@@ -1029,7 +1071,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="60">
   <si>
     <t>exp024_michael lactate timecourse</t>
   </si>
@@ -1200,6 +1242,15 @@
   </si>
   <si>
     <t>unknown</t>
+  </si>
+  <si>
+    <t>Animal Treatment</t>
+  </si>
+  <si>
+    <t>Treatment Description</t>
+  </si>
+  <si>
+    <t>For protocol's full text, please consult Michael Neinast.</t>
   </si>
 </sst>
 </file>
@@ -1315,7 +1366,59 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{6B4086E8-9FD8-334C-AC15-A184A522FCB0}"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="17">
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDCE6F1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -2243,17 +2346,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:E1">
-    <cfRule type="notContainsErrors" dxfId="14" priority="1">
+    <cfRule type="notContainsErrors" dxfId="16" priority="1">
       <formula>NOT(ISERROR(A1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1">
-    <cfRule type="notContainsErrors" dxfId="13" priority="2">
+    <cfRule type="notContainsErrors" dxfId="15" priority="2">
       <formula>NOT(ISERROR(F1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1">
-    <cfRule type="notContainsErrors" dxfId="12" priority="3">
+    <cfRule type="notContainsErrors" dxfId="14" priority="3">
       <formula>NOT(ISERROR(G1))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2421,22 +2524,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1">
-    <cfRule type="notContainsErrors" dxfId="11" priority="1">
+    <cfRule type="notContainsErrors" dxfId="13" priority="1">
       <formula>NOT(ISERROR(A1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1">
-    <cfRule type="notContainsErrors" dxfId="10" priority="2">
+    <cfRule type="notContainsErrors" dxfId="12" priority="2">
       <formula>NOT(ISERROR(B1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:D1">
-    <cfRule type="notContainsErrors" dxfId="9" priority="3">
+    <cfRule type="notContainsErrors" dxfId="11" priority="3">
       <formula>NOT(ISERROR(C1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1">
-    <cfRule type="notContainsErrors" dxfId="8" priority="4">
+    <cfRule type="notContainsErrors" dxfId="10" priority="4">
       <formula>NOT(ISERROR(E1))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2547,12 +2650,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:G1">
-    <cfRule type="notContainsErrors" dxfId="7" priority="1">
+    <cfRule type="notContainsErrors" dxfId="9" priority="1">
       <formula>NOT(ISERROR(A1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:K1">
-    <cfRule type="notContainsErrors" dxfId="6" priority="2">
+    <cfRule type="notContainsErrors" dxfId="8" priority="2">
       <formula>NOT(ISERROR(C1))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2701,17 +2804,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:D1">
-    <cfRule type="notContainsErrors" dxfId="5" priority="1">
+    <cfRule type="notContainsErrors" dxfId="7" priority="1">
       <formula>NOT(ISERROR(A1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1">
-    <cfRule type="notContainsErrors" dxfId="4" priority="2">
+    <cfRule type="notContainsErrors" dxfId="6" priority="2">
       <formula>NOT(ISERROR(E1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1">
-    <cfRule type="notContainsErrors" dxfId="3" priority="3">
+    <cfRule type="notContainsErrors" dxfId="5" priority="3">
       <formula>NOT(ISERROR(F1))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2724,7 +2827,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F123856A-408E-3545-8A33-14C15BE5C60F}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -2899,17 +3002,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1">
-    <cfRule type="notContainsErrors" dxfId="2" priority="1">
+    <cfRule type="notContainsErrors" dxfId="4" priority="1">
       <formula>NOT(ISERROR(A1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:E1">
-    <cfRule type="notContainsErrors" dxfId="1" priority="2">
+    <cfRule type="notContainsErrors" dxfId="3" priority="2">
       <formula>NOT(ISERROR(B1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1">
-    <cfRule type="notContainsErrors" dxfId="0" priority="3">
+    <cfRule type="notContainsErrors" dxfId="2" priority="3">
       <formula>NOT(ISERROR(F1))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2924,4 +3027,51 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAC62062-D06C-C946-9F5F-76160532E31A}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="17" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1">
+    <cfRule type="notContainsErrors" dxfId="1" priority="1">
+      <formula>NOT(ISERROR(A1))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1">
+    <cfRule type="notContainsErrors" dxfId="0" priority="2">
+      <formula>NOT(ISERROR(B1))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>